<commit_message>
Adición de limpieza de datos biológicos
</commit_message>
<xml_diff>
--- a/01_Analisis_Exploratorio/02_Datos/Biologicos/DatosP_Fitoplancton/Event_ID_EXP.PACÍFICO_2021.xlsx
+++ b/01_Analisis_Exploratorio/02_Datos/Biologicos/DatosP_Fitoplancton/Event_ID_EXP.PACÍFICO_2021.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Expedicion_Pacifico\2021\Ictioplancton\Analisis_Exp_Pac\Ictioplancton_ExPacifico2020\01_Analisis_Exploratorio\02_Datos\Biologicos\DarwinCore\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Expedicion_Pacifico\2021\Ictioplancton\Analisis_Exp_Pac\Ictioplancton_ExPacifico2020\01_Analisis_Exploratorio\02_Datos\Biologicos\DatosP_Fitoplancton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71EFFD3-DADC-4609-AF83-A0D2DAAC3B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5718F0B4-C089-40D0-8D07-252F530487A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="2" r:id="rId1"/>
@@ -1388,11 +1388,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Hoja1"/>
+  <sheetPr codeName="Hoja1" filterMode="1"/>
   <dimension ref="A1:V75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="T34" sqref="T34:T73"/>
@@ -1493,7 +1493,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>33</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>34</v>
       </c>
@@ -1945,7 +1945,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>35</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>37</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>38</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>39</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>40</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>41</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>42</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>43</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>44</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>45</v>
       </c>
@@ -3177,7 +3177,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>46</v>
       </c>
@@ -3289,7 +3289,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>47</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>48</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>49</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>50</v>
       </c>
@@ -3737,7 +3737,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>51</v>
       </c>
@@ -3849,7 +3849,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>52</v>
       </c>
@@ -3961,7 +3961,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>53</v>
       </c>
@@ -4073,7 +4073,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>54</v>
       </c>
@@ -4185,7 +4185,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>55</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>56</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>57</v>
       </c>
@@ -4521,7 +4521,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>58</v>
       </c>
@@ -4633,7 +4633,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>59</v>
       </c>
@@ -4745,7 +4745,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>60</v>
       </c>
@@ -4857,7 +4857,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>61</v>
       </c>
@@ -4969,7 +4969,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>62</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>63</v>
       </c>
@@ -5193,7 +5193,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>64</v>
       </c>
@@ -5305,7 +5305,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>65</v>
       </c>
@@ -5417,7 +5417,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>66</v>
       </c>
@@ -5535,7 +5535,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V73" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:V73" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="Red Bongo, arrastre superficial 300 &amp; 500µm"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="24" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>